<commit_message>
updated XLSX to force gene lists
</commit_message>
<xml_diff>
--- a/inst/extdata/heatmap_genes.xlsx
+++ b/inst/extdata/heatmap_genes.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">synapse organization </t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0050808</t>
+    <t xml:space="preserve">forced.GO:0050808</t>
   </si>
   <si>
     <t xml:space="preserve">APOE</t>
@@ -148,6 +148,24 @@
     <t xml:space="preserve">GO:0050804</t>
   </si>
   <si>
+    <t xml:space="preserve">chemical synaptic transmission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0007268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positive regulation of vasculature development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:1904018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation of angiogenesis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forced.GO:0045765</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMILIN1</t>
   </si>
   <si>
@@ -206,24 +224,6 @@
   </si>
   <si>
     <t xml:space="preserve">BTG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chemical synaptic transmission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0007268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">positive regulation of vasculature development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:1904018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regulation of angiogenesis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0045765</t>
   </si>
   <si>
     <t xml:space="preserve">astrocyte identity</t>
@@ -1118,9 +1118,9 @@
   <dimension ref="A1:AQ37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1284,82 +1284,16 @@
       <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="S7" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="U7" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="X7" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y7" s="0" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1367,20 +1301,86 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="X10" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="Y10" s="0" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
         <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>98</v>
@@ -1816,7 +1816,7 @@
         <v>181</v>
       </c>
       <c r="AF25" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="AG25" s="1" t="s">
         <v>182</v>

</xml_diff>